<commit_message>
fixed some qa errors
</commit_message>
<xml_diff>
--- a/models-src/hl7-eps-models-and-maps.xlsx
+++ b/models-src/hl7-eps-models-and-maps.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\___Python\fsh-excel-fsh\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\hl7eu-eps\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AB117C-BACC-4509-9A90-EB9ECC236F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC2250C-1046-46B0-A2B6-BD6706C2CF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="669">
   <si>
     <t>Group Source</t>
   </si>
@@ -1889,12 +1889,6 @@
     <t>TargetUri</t>
   </si>
   <si>
-    <t>patientSummary2FHIR-eu-ps</t>
-  </si>
-  <si>
-    <t>subject2FHIR-eu-ps</t>
-  </si>
-  <si>
     <t>PatientSummary2FHIR</t>
   </si>
   <si>
@@ -2062,23 +2056,26 @@
     <t>http://hl7.eu/fhir/eps/StructureDefinition/Patient-ps-xpandh</t>
   </si>
   <si>
-    <t>http://hl7.eu/fhir/eps/StructureDefinition/Bundle-eu-ps</t>
-  </si>
-  <si>
-    <t>http://hl7.eu/fhir/eps/StructureDefinition/Bundle-ps-xpandh</t>
-  </si>
-  <si>
-    <t>http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR-eu-ps</t>
-  </si>
-  <si>
-    <t>http://hl7.eu/fhir/eps/ConceptMap/subject2FHIR-eu-ps</t>
+    <t>http://hl7.eu/fhir/eps/StructureDefinition/Bundle-eu-eps</t>
+  </si>
+  <si>
+    <t>patientSummary2FHIR</t>
+  </si>
+  <si>
+    <t>subjectPs2FHIR</t>
+  </si>
+  <si>
+    <t>Experimental</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2100,6 +2097,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2141,7 +2144,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2160,6 +2163,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -2511,10 +2515,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
@@ -2535,10 +2539,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
@@ -2559,10 +2563,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
@@ -2583,10 +2587,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
@@ -2607,10 +2611,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>7</v>
@@ -2631,10 +2635,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>8</v>
@@ -2655,10 +2659,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>9</v>
@@ -2679,10 +2683,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>9</v>
@@ -2703,10 +2707,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>10</v>
@@ -2727,10 +2731,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>11</v>
@@ -2751,10 +2755,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>12</v>
@@ -2775,10 +2779,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>13</v>
@@ -2799,10 +2803,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>14</v>
@@ -2823,10 +2827,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>15</v>
@@ -2847,10 +2851,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>16</v>
@@ -2871,10 +2875,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>17</v>
@@ -2895,10 +2899,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A18" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>18</v>
@@ -2917,10 +2921,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>19</v>
@@ -2939,10 +2943,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A20" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>20</v>
@@ -2961,10 +2965,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A21" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>21</v>
@@ -2983,10 +2987,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A22" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>21</v>
@@ -3005,10 +3009,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A23" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>22</v>
@@ -3027,10 +3031,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A24" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>23</v>
@@ -3049,10 +3053,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A25" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>24</v>
@@ -3071,10 +3075,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A26" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>25</v>
@@ -3093,10 +3097,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A27" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>26</v>
@@ -3115,10 +3119,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A28" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>27</v>
@@ -3137,10 +3141,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A29" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>28</v>
@@ -3159,10 +3163,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A30" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>29</v>
@@ -3181,10 +3185,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A31" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>30</v>
@@ -3203,10 +3207,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A32" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>31</v>
@@ -3225,10 +3229,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A33" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>32</v>
@@ -3247,10 +3251,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A34" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>33</v>
@@ -3269,10 +3273,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A35" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>34</v>
@@ -3291,10 +3295,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A36" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>35</v>
@@ -3313,10 +3317,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A37" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>36</v>
@@ -3335,10 +3339,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A38" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>37</v>
@@ -3357,10 +3361,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A39" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>38</v>
@@ -3379,10 +3383,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A40" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>39</v>
@@ -3401,10 +3405,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A41" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>40</v>
@@ -3423,10 +3427,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A42" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>41</v>
@@ -3445,10 +3449,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A43" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>40</v>
@@ -3467,10 +3471,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A44" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>41</v>
@@ -3489,10 +3493,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A45" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>42</v>
@@ -3511,10 +3515,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A46" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>43</v>
@@ -3533,10 +3537,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A47" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>44</v>
@@ -3555,10 +3559,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A48" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>45</v>
@@ -3577,10 +3581,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A49" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>46</v>
@@ -3599,10 +3603,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A50" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>14</v>
@@ -3619,10 +3623,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A51" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>15</v>
@@ -3639,10 +3643,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A52" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>16</v>
@@ -4852,10 +4856,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C2" t="s">
         <v>530</v>
@@ -4875,10 +4879,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="C3" t="s">
         <v>531</v>
@@ -4898,10 +4902,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C4" t="s">
         <v>532</v>
@@ -4921,10 +4925,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C5" t="s">
         <v>533</v>
@@ -4944,10 +4948,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C6" t="s">
         <v>534</v>
@@ -4967,10 +4971,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C7" t="s">
         <v>535</v>
@@ -4990,10 +4994,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C8" t="s">
         <v>536</v>
@@ -5013,10 +5017,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C9" t="s">
         <v>537</v>
@@ -5036,10 +5040,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C10" t="s">
         <v>538</v>
@@ -5059,10 +5063,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C11" t="s">
         <v>539</v>
@@ -5082,10 +5086,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C12" t="s">
         <v>539</v>
@@ -5105,10 +5109,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C13" t="s">
         <v>540</v>
@@ -5128,10 +5132,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C14" t="s">
         <v>541</v>
@@ -5151,10 +5155,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C15" t="s">
         <v>542</v>
@@ -5174,10 +5178,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C16" t="s">
         <v>543</v>
@@ -5197,10 +5201,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C17" t="s">
         <v>544</v>
@@ -5220,10 +5224,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A18" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C18" t="s">
         <v>544</v>
@@ -5240,10 +5244,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C19" t="s">
         <v>545</v>
@@ -5260,10 +5264,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A20" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C20" t="s">
         <v>546</v>
@@ -5280,10 +5284,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A21" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C21" t="s">
         <v>547</v>
@@ -5300,10 +5304,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A22" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C22" t="s">
         <v>548</v>
@@ -5320,10 +5324,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A23" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C23" t="s">
         <v>549</v>
@@ -5340,10 +5344,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A24" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C24" t="s">
         <v>550</v>
@@ -5360,10 +5364,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A25" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C25" t="s">
         <v>551</v>
@@ -5380,10 +5384,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A26" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C26" t="s">
         <v>552</v>
@@ -5400,10 +5404,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A27" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C27" t="s">
         <v>553</v>
@@ -5420,10 +5424,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A28" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C28" t="s">
         <v>554</v>
@@ -5440,10 +5444,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A29" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C29" t="s">
         <v>530</v>
@@ -5460,10 +5464,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A30" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C30" t="s">
         <v>547</v>
@@ -5480,10 +5484,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A31" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C31" t="s">
         <v>555</v>
@@ -5500,10 +5504,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A32" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C32" t="s">
         <v>556</v>
@@ -5520,10 +5524,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A33" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C33" t="s">
         <v>557</v>
@@ -5540,10 +5544,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A34" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C34" t="s">
         <v>558</v>
@@ -5560,10 +5564,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A35" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C35" t="s">
         <v>559</v>
@@ -5580,10 +5584,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A36" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C36" t="s">
         <v>560</v>
@@ -5600,10 +5604,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A37" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C37" t="s">
         <v>561</v>
@@ -5698,10 +5702,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I1" sqref="I1:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -5714,7 +5718,7 @@
     <col min="8" max="8" width="61.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
         <v>601</v>
       </c>
@@ -5739,70 +5743,79 @@
       <c r="H1" s="2" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="I1" s="2" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
+        <v>665</v>
+      </c>
+      <c r="B2" t="s">
         <v>609</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="str">
+        <f>"http://hl7.eu/fhir/eps/ConceptMap/"&amp;A2</f>
+        <v>http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR</v>
+      </c>
+      <c r="D2" t="s">
         <v>611</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" t="s">
+        <v>611</v>
+      </c>
+      <c r="F2" t="s">
+        <v>614</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="I2" t="s">
         <v>668</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>666</v>
+      </c>
+      <c r="B3" t="s">
+        <v>610</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>"http://hl7.eu/fhir/eps/ConceptMap/"&amp;A3</f>
+        <v>http://hl7.eu/fhir/eps/ConceptMap/subjectPs2FHIR</v>
+      </c>
+      <c r="D3" t="s">
+        <v>612</v>
+      </c>
+      <c r="E3" t="s">
         <v>613</v>
       </c>
-      <c r="E2" t="s">
-        <v>613</v>
-      </c>
-      <c r="F2" t="s">
-        <v>616</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>610</v>
-      </c>
-      <c r="B3" t="s">
-        <v>612</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>614</v>
       </c>
-      <c r="E3" t="s">
-        <v>615</v>
-      </c>
-      <c r="F3" t="s">
-        <v>616</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+        <v>656</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="I3" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.75">
       <c r="C12" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="http://hl7.eu/fhir/ig/xpandh/ps/StructureDefinition/PatientSummary" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
-    <hyperlink ref="H2" r:id="rId2" display="http://hl7.eu/fhir/ig/xpandh/ps/StructureDefinition/Bundle-eu-ps" xr:uid="{00000000-0004-0000-0E00-000002000000}"/>
-    <hyperlink ref="G3" r:id="rId3" display="http://hl7.eu/fhir/ig/xpandh/ps/StructureDefinition/Subject" xr:uid="{00000000-0004-0000-0E00-000004000000}"/>
-    <hyperlink ref="H3" r:id="rId4" display="http://hl7.eu/fhir/ig/xpandh/ps/StructureDefinition/Bundle-ps-xpandh" xr:uid="{00000000-0004-0000-0E00-000005000000}"/>
-    <hyperlink ref="C3" r:id="rId5" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{00000000-0004-0000-0E00-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId6" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" display="http://hl7.eu/fhir/ig/xpandh/ps/StructureDefinition/Subject" xr:uid="{00000000-0004-0000-0E00-000004000000}"/>
+    <hyperlink ref="C2" r:id="rId3" display="http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId4" display="http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR" xr:uid="{0041CA32-1BC1-4938-801E-686765723E3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5826,7 +5839,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>602</v>
@@ -5840,24 +5853,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2" s="5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A3" s="5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>221</v>
@@ -5868,142 +5881,142 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A4" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>226</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A5" s="5" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>229</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A6" s="5" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A7" s="5" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A8" s="5" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A9" s="5" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>73</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A10" s="5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>230</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A11" s="5" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>243</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A12" s="5" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A13" s="5" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>225</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
   </sheetData>
@@ -6070,7 +6083,7 @@
         <v>197</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>49</v>
@@ -6325,7 +6338,7 @@
         <v>199</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>64</v>
@@ -6393,7 +6406,7 @@
         <v>199</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>68</v>
@@ -6410,7 +6423,7 @@
         <v>199</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>69</v>
@@ -6478,7 +6491,7 @@
         <v>198</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>73</v>
@@ -6563,7 +6576,7 @@
         <v>200</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>78</v>
@@ -6750,7 +6763,7 @@
         <v>198</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
added dependency from eu base
</commit_message>
<xml_diff>
--- a/models-src/hl7-eps-models-and-maps.xlsx
+++ b/models-src/hl7-eps-models-and-maps.xlsx
@@ -8,28 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\hl7eu-eps\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF1CAE0-4F6E-4BBE-A6EC-33A11E94B7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2F38C0-10F5-4A88-AF72-B2DC27F9481F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConceptMaps" sheetId="15" r:id="rId1"/>
     <sheet name="PatientSummary2FHIR" sheetId="1" r:id="rId2"/>
     <sheet name="PatientSummarySubject2Fhir" sheetId="14" r:id="rId3"/>
     <sheet name="PatientSummaryEhn" sheetId="2" r:id="rId4"/>
-    <sheet name="AllergyPsEhn" sheetId="3" r:id="rId5"/>
-    <sheet name="ClosedProblemPsEhn" sheetId="4" r:id="rId6"/>
-    <sheet name="MedicalDevicePsEhn" sheetId="5" r:id="rId7"/>
-    <sheet name="FunctionalStatusPsEhn" sheetId="6" r:id="rId8"/>
-    <sheet name="MedicinePsEhn" sheetId="7" r:id="rId9"/>
-    <sheet name="PregnancyPsEhn" sheetId="8" r:id="rId10"/>
-    <sheet name="ProblemPsEhn" sheetId="9" r:id="rId11"/>
-    <sheet name="ProcedurePsEhn" sheetId="10" r:id="rId12"/>
-    <sheet name="ResultPsEhn" sheetId="11" r:id="rId13"/>
-    <sheet name="SubjectPsEhn" sheetId="12" r:id="rId14"/>
-    <sheet name="VaccinationPsEhn" sheetId="13" r:id="rId15"/>
-    <sheet name="LogicalModels" sheetId="16" r:id="rId16"/>
+    <sheet name="Alerts2FHIREuHdr" sheetId="17" r:id="rId5"/>
+    <sheet name="AllergyPsEhn" sheetId="3" r:id="rId6"/>
+    <sheet name="ClosedProblemPsEhn" sheetId="4" r:id="rId7"/>
+    <sheet name="MedicalDevicePsEhn" sheetId="5" r:id="rId8"/>
+    <sheet name="FunctionalStatusPsEhn" sheetId="6" r:id="rId9"/>
+    <sheet name="MedicinePsEhn" sheetId="7" r:id="rId10"/>
+    <sheet name="PregnancyPsEhn" sheetId="8" r:id="rId11"/>
+    <sheet name="ProblemPsEhn" sheetId="9" r:id="rId12"/>
+    <sheet name="ProcedurePsEhn" sheetId="10" r:id="rId13"/>
+    <sheet name="ResultPsEhn" sheetId="11" r:id="rId14"/>
+    <sheet name="SubjectPsEhn" sheetId="12" r:id="rId15"/>
+    <sheet name="VaccinationPsEhn" sheetId="13" r:id="rId16"/>
+    <sheet name="LogicalModels" sheetId="16" r:id="rId17"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="CENEN13606Lekarska_prepustacia_sprava">'[2]Hospital Discharge Report '!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -48,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="707">
   <si>
     <t>Group Source</t>
   </si>
@@ -1838,12 +1846,6 @@
     <t>TargetUri</t>
   </si>
   <si>
-    <t>PatientSummary2FHIR</t>
-  </si>
-  <si>
-    <t>PatientSummarySubject2Fhir</t>
-  </si>
-  <si>
     <t>eHN Patient Summary to this guide Map</t>
   </si>
   <si>
@@ -1999,16 +2001,7 @@
     <t>http://hl7.eu/fhir/eps/StructureDefinition/Bundle-eu-eps</t>
   </si>
   <si>
-    <t>patientSummary2FHIR</t>
-  </si>
-  <si>
-    <t>subjectPs2FHIR</t>
-  </si>
-  <si>
     <t>Experimental</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
   <si>
     <t>Allergy. Section A.2.1.1</t>
@@ -2100,6 +2093,105 @@
   </si>
   <si>
     <t>to be checked be sure is not mapped in the IPS Patient Story</t>
+  </si>
+  <si>
+    <t>eHN Alerts Model to this guide Map</t>
+  </si>
+  <si>
+    <t>eHN HDR Alerts Model to this guide mapping</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>patientSummary2FHIR-eu-eps</t>
+  </si>
+  <si>
+    <t>subject2FHIR-eu-eps</t>
+  </si>
+  <si>
+    <t>alerts2FHIR-eu-eps</t>
+  </si>
+  <si>
+    <t>Subject2FhirEuPs</t>
+  </si>
+  <si>
+    <t>Alerts2FHIREuPs</t>
+  </si>
+  <si>
+    <t>PatientSummary2FHIREuPs</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/eps/StructureDefinition/Alert</t>
+  </si>
+  <si>
+    <t>Composition.section:sectionAllergies</t>
+  </si>
+  <si>
+    <t>relatedto</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance</t>
+  </si>
+  <si>
+    <t>equivalent</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.text</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.type</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.reaction</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.reaction.manifestation</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.reaction.severity</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.criticality</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.onsetDateTime</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.extension:abatement-datetime</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.clinicalStatus</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.verificationStatus</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance.code</t>
+  </si>
+  <si>
+    <t>Composition.section:sectionAlerts</t>
+  </si>
+  <si>
+    <t>Composition.section:sectionAlerts.text</t>
+  </si>
+  <si>
+    <t>Flag.text</t>
+  </si>
+  <si>
+    <t>Flag.code.text</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-eps</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/hdr/StructureDefinition/allergyIntolerance-eu-eps</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/eps/StructureDefinition/Alerts</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/hdr/StructureDefinition/flag-eu-eps</t>
   </si>
 </sst>
 </file>
@@ -2249,6 +2341,241 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="ConceptMaps"/>
+      <sheetName val="LogicalModels"/>
+      <sheetName val="Alerts2FHIREuHdr"/>
+      <sheetName val="AlertsEhn"/>
+      <sheetName val="Encounter2FHIREuHdr"/>
+      <sheetName val="Header2FHIREuHdr"/>
+      <sheetName val="HeaderHdrEhn"/>
+      <sheetName val="Subject2FHIREuHdr"/>
+      <sheetName val="SubjectHdrEhn"/>
+      <sheetName val="AdmissionEvaluationEhn"/>
+      <sheetName val="AdvanceDirectivesEhn"/>
+      <sheetName val="DischargeDetailsEhn"/>
+      <sheetName val="EncounterEhn"/>
+      <sheetName val="HospitalStayEhn"/>
+      <sheetName val="PatientHistoryEhn"/>
+      <sheetName val="RecommendationsEhn"/>
+      <sheetName val="HospitalDischargeReportEhn"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>allergy</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>A.2.2.1 - Allergy and Intolerance</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>allergy.description</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>A.2.2.1.1 - Allergy description</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>allergy.typeOfPropensity</v>
+          </cell>
+          <cell r="D4" t="str">
+            <v>A.2.2.1.2 - Type of propensity</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>allergy.manifestation</v>
+          </cell>
+          <cell r="D5" t="str">
+            <v>A.2.2.1.3 - Allergy manifestation</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>allergy.severity</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>A.2.2.1.4 - Severity</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>allergy.criticality</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>A.2.2.1.5 - Criticality</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>allergy.onsetDate</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>A.2.2.1.6 - Onset date</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>allergy.endDate</v>
+          </cell>
+          <cell r="D11" t="str">
+            <v>A.2.2.1.7 - End date</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>allergy.status</v>
+          </cell>
+          <cell r="D14" t="str">
+            <v>A.2.2.1.8 - Status</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>allergy.certainty</v>
+          </cell>
+          <cell r="D15" t="str">
+            <v>A.2.2.1.9 - Certainty</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>allergy.agent</v>
+          </cell>
+          <cell r="D16" t="str">
+            <v>A.2.2.1.10 - Agent or Allergen</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>medicalAlerts</v>
+          </cell>
+          <cell r="D17" t="str">
+            <v>A.2.2.2 - Medical alerts (relevant for the respective hospital stay)</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>medicalAlerts.description</v>
+          </cell>
+          <cell r="D18" t="str">
+            <v>A.2.2.2.1 - Healthcare alert description</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Hospital Discharge Report "/>
+      <sheetName val="HospitalDischargeReport"/>
+      <sheetName val="HospitalDischargeReport-Map-1"/>
+      <sheetName val="HospitalDischargeReport-fsh"/>
+      <sheetName val="HospitalDischargeRep-ConceptMap"/>
+      <sheetName val="HospitalDischargeReport-CM-fsh"/>
+      <sheetName val="HDR-SK"/>
+      <sheetName val="HospitalDischargeReportSK"/>
+      <sheetName val="HospitalDischargeReportSK-Map"/>
+      <sheetName val="HospitalDischargeReportSK-fsh"/>
+      <sheetName val="Subject"/>
+      <sheetName val="Subject-Map-1"/>
+      <sheetName val="Subject-fsh"/>
+      <sheetName val="Subject-ConceptMap"/>
+      <sheetName val="Subject-CM-fsh"/>
+      <sheetName val="Staging"/>
+      <sheetName val="Staging-Map-1"/>
+      <sheetName val="Staging-fsh"/>
+      <sheetName val="Staging-ConceptMap"/>
+      <sheetName val="Staging-CM-fsh"/>
+      <sheetName val="Treatment"/>
+      <sheetName val="Treatment-Map-1"/>
+      <sheetName val="Treatment-fsh"/>
+      <sheetName val="Treatment-ConceptMap"/>
+      <sheetName val="Treatment-CM-fsh"/>
+      <sheetName val="ConvertOsiris"/>
+      <sheetName val="Osiris"/>
+      <sheetName val="Osiris-Map"/>
+      <sheetName val="Osiris-fsh-noMap"/>
+      <sheetName val="Osiris-fsh"/>
+      <sheetName val="Osiris-ConceptMap"/>
+      <sheetName val="Osiris-CM-fsh"/>
+      <sheetName val="Foglio2"/>
+      <sheetName val="xpandh-hdr-model-maps"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2544,7 +2871,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2583,67 +2910,97 @@
         <v>591</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>645</v>
+        <v>677</v>
       </c>
       <c r="B2" t="s">
-        <v>592</v>
+        <v>682</v>
       </c>
       <c r="C2" s="1" t="str">
         <f>"http://hl7.eu/fhir/eps/ConceptMap/"&amp;A2</f>
-        <v>http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR</v>
+        <v>http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR-eu-eps</v>
       </c>
       <c r="D2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="E2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F2" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="I2" t="s">
-        <v>648</v>
+        <v>642</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>646</v>
+        <v>678</v>
       </c>
       <c r="B3" t="s">
-        <v>593</v>
+        <v>680</v>
       </c>
       <c r="C3" s="1" t="str">
         <f>"http://hl7.eu/fhir/eps/ConceptMap/"&amp;A3</f>
-        <v>http://hl7.eu/fhir/eps/ConceptMap/subjectPs2FHIR</v>
+        <v>http://hl7.eu/fhir/eps/ConceptMap/subject2FHIR-eu-eps</v>
       </c>
       <c r="D3" t="s">
+        <v>593</v>
+      </c>
+      <c r="E3" t="s">
+        <v>594</v>
+      </c>
+      <c r="F3" t="s">
         <v>595</v>
       </c>
-      <c r="E3" t="s">
-        <v>596</v>
-      </c>
-      <c r="F3" t="s">
-        <v>597</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>644</v>
-      </c>
-      <c r="I3" t="s">
+        <v>642</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A4" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="C4" s="8" t="str">
+        <f t="shared" ref="C4" si="0">"http://hl7.eu/fhir/hdr/ConceptMap/"&amp;A4</f>
+        <v>http://hl7.eu/fhir/hdr/ConceptMap/alerts2FHIR-eu-eps</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>648</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.75">
@@ -2655,12 +3012,198 @@
     <hyperlink ref="G3" r:id="rId2" display="http://hl7.eu/fhir/ig/xpandh/ps/StructureDefinition/Subject" xr:uid="{00000000-0004-0000-0E00-000004000000}"/>
     <hyperlink ref="C2" r:id="rId3" display="http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
     <hyperlink ref="C3" r:id="rId4" display="http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR" xr:uid="{0041CA32-1BC1-4938-801E-686765723E3F}"/>
+    <hyperlink ref="C4" r:id="rId5" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{42BB9F16-F29B-4D9B-A55C-529961F089C2}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{D0CFA2F1-ED0F-4899-907A-300DECE34DC2}"/>
+    <hyperlink ref="G4" r:id="rId7" xr:uid="{D6CB4B67-C29F-4503-B9BB-BD22D2DA2E6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" t="s">
+        <v>306</v>
+      </c>
+      <c r="E2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" t="s">
+        <v>299</v>
+      </c>
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B6" t="s">
+        <v>300</v>
+      </c>
+      <c r="C6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D7" t="s">
+        <v>311</v>
+      </c>
+      <c r="E7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>297</v>
+      </c>
+      <c r="B8" t="s">
+        <v>302</v>
+      </c>
+      <c r="C8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" t="s">
+        <v>312</v>
+      </c>
+      <c r="E8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B9" t="s">
+        <v>303</v>
+      </c>
+      <c r="C9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10" t="s">
+        <v>304</v>
+      </c>
+      <c r="C10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10" t="s">
+        <v>314</v>
+      </c>
+      <c r="E10" t="s">
+        <v>323</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -2860,7 +3403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2941,7 +3484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3022,7 +3565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -3188,7 +3731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
@@ -3745,7 +4288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -3979,7 +4522,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -3997,7 +4540,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>585</v>
@@ -4011,170 +4554,170 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A2" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A3" s="5" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>204</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A4" s="5" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>209</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A5" s="5" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>212</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A6" s="5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="44.25" x14ac:dyDescent="0.75">
       <c r="A7" s="5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A8" s="5" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>81</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A9" s="5" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>72</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A10" s="5" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>213</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A11" s="5" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>226</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A12" s="5" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A13" s="5" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>208</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -4192,7 +4735,7 @@
   </sheetPr>
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="C18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -4236,10 +4779,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>3</v>
@@ -4257,10 +4800,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>4</v>
@@ -4278,10 +4821,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -4297,15 +4840,15 @@
         <v>125</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
@@ -4323,10 +4866,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
@@ -4342,15 +4885,15 @@
         <v>125</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>7</v>
@@ -4368,10 +4911,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>8</v>
@@ -4380,22 +4923,22 @@
         <v>52</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="15" t="s">
         <v>124</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>8</v>
@@ -4411,15 +4954,15 @@
         <v>124</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>9</v>
@@ -4435,15 +4978,15 @@
         <v>124</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>9</v>
@@ -4464,10 +5007,10 @@
     </row>
     <row r="12" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A12" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>10</v>
@@ -4488,10 +5031,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>11</v>
@@ -4509,10 +5052,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>12</v>
@@ -4528,18 +5071,18 @@
         <v>125</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>57</v>
@@ -4557,10 +5100,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>13</v>
@@ -4578,10 +5121,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>14</v>
@@ -4599,10 +5142,10 @@
     </row>
     <row r="18" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A18" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>15</v>
@@ -4618,15 +5161,15 @@
         <v>124</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>16</v>
@@ -4644,10 +5187,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A20" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>17</v>
@@ -4663,15 +5206,15 @@
         <v>124</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A21" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>18</v>
@@ -4689,10 +5232,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A22" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>19</v>
@@ -4710,10 +5253,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A23" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>20</v>
@@ -4731,10 +5274,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A24" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>20</v>
@@ -4743,22 +5286,22 @@
         <v>65</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="15" t="s">
         <v>124</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A25" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>20</v>
@@ -4767,22 +5310,22 @@
         <v>65</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="15" t="s">
         <v>124</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A26" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>21</v>
@@ -4798,15 +5341,15 @@
         <v>124</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A27" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>22</v>
@@ -4827,10 +5370,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A28" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>23</v>
@@ -4848,10 +5391,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A29" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>24</v>
@@ -4860,22 +5403,22 @@
         <v>69</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="15" t="s">
         <v>124</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A30" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>25</v>
@@ -4884,7 +5427,7 @@
         <v>70</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="15" t="s">
@@ -4894,10 +5437,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A31" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>26</v>
@@ -4915,10 +5458,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A32" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>27</v>
@@ -4927,7 +5470,7 @@
         <v>72</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="15" t="s">
@@ -4936,10 +5479,10 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A33" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>28</v>
@@ -4957,10 +5500,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A34" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>29</v>
@@ -4978,10 +5521,10 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A35" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>30</v>
@@ -4999,10 +5542,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A36" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>31</v>
@@ -5020,10 +5563,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A37" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>32</v>
@@ -5041,10 +5584,10 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A38" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>33</v>
@@ -5062,10 +5605,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A39" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>34</v>
@@ -5081,15 +5624,15 @@
         <v>125</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A40" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>35</v>
@@ -5105,15 +5648,15 @@
         <v>125</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A41" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>36</v>
@@ -5131,10 +5674,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A42" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>37</v>
@@ -5150,15 +5693,15 @@
         <v>124</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A43" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>38</v>
@@ -5176,10 +5719,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A44" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>39</v>
@@ -5197,10 +5740,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A45" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>40</v>
@@ -5218,10 +5761,10 @@
     </row>
     <row r="46" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A46" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>39</v>
@@ -5230,22 +5773,22 @@
         <v>84</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="F46" s="5"/>
       <c r="G46" s="15" t="s">
         <v>124</v>
       </c>
       <c r="H46" s="17" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A47" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>40</v>
@@ -5254,22 +5797,22 @@
         <v>85</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="F47" s="5"/>
       <c r="G47" s="15" t="s">
         <v>124</v>
       </c>
       <c r="H47" s="17" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A48" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>41</v>
@@ -5287,10 +5830,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A49" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>42</v>
@@ -5308,10 +5851,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A50" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>43</v>
@@ -5329,10 +5872,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A51" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>44</v>
@@ -5350,10 +5893,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A52" s="8" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>45</v>
@@ -5459,7 +6002,7 @@
   </sheetPr>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B37"/>
     </sheetView>
   </sheetViews>
@@ -5503,10 +6046,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C2" t="s">
         <v>513</v>
@@ -5526,10 +6069,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C3" t="s">
         <v>514</v>
@@ -5549,10 +6092,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C4" t="s">
         <v>515</v>
@@ -5572,10 +6115,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C5" t="s">
         <v>516</v>
@@ -5595,10 +6138,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C6" t="s">
         <v>517</v>
@@ -5618,10 +6161,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C7" t="s">
         <v>518</v>
@@ -5641,10 +6184,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A8" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C8" t="s">
         <v>519</v>
@@ -5664,10 +6207,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A9" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C9" t="s">
         <v>520</v>
@@ -5687,10 +6230,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C10" t="s">
         <v>521</v>
@@ -5710,10 +6253,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A11" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C11" t="s">
         <v>522</v>
@@ -5733,10 +6276,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A12" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C12" t="s">
         <v>522</v>
@@ -5756,10 +6299,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A13" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C13" t="s">
         <v>523</v>
@@ -5779,10 +6322,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A14" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C14" t="s">
         <v>524</v>
@@ -5802,10 +6345,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A15" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C15" t="s">
         <v>525</v>
@@ -5825,10 +6368,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A16" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C16" t="s">
         <v>526</v>
@@ -5848,10 +6391,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A17" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C17" t="s">
         <v>527</v>
@@ -5871,10 +6414,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A18" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C18" t="s">
         <v>527</v>
@@ -5891,10 +6434,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A19" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C19" t="s">
         <v>528</v>
@@ -5911,10 +6454,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A20" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C20" t="s">
         <v>529</v>
@@ -5931,10 +6474,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A21" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C21" t="s">
         <v>530</v>
@@ -5951,10 +6494,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A22" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C22" t="s">
         <v>531</v>
@@ -5971,10 +6514,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A23" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C23" t="s">
         <v>532</v>
@@ -5991,10 +6534,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A24" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C24" t="s">
         <v>533</v>
@@ -6011,10 +6554,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A25" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C25" t="s">
         <v>534</v>
@@ -6031,10 +6574,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A26" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C26" t="s">
         <v>535</v>
@@ -6051,10 +6594,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A27" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C27" t="s">
         <v>536</v>
@@ -6071,10 +6614,10 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A28" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C28" t="s">
         <v>537</v>
@@ -6091,10 +6634,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A29" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C29" t="s">
         <v>513</v>
@@ -6111,10 +6654,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A30" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C30" t="s">
         <v>530</v>
@@ -6131,10 +6674,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A31" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C31" t="s">
         <v>538</v>
@@ -6151,10 +6694,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A32" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C32" t="s">
         <v>539</v>
@@ -6171,10 +6714,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A33" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C33" t="s">
         <v>540</v>
@@ -6191,10 +6734,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A34" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C34" t="s">
         <v>541</v>
@@ -6211,10 +6754,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A35" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C35" t="s">
         <v>542</v>
@@ -6231,10 +6774,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A36" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C36" t="s">
         <v>543</v>
@@ -6251,10 +6794,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A37" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="C37" t="s">
         <v>544</v>
@@ -6376,7 +6919,7 @@
         <v>180</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>48</v>
@@ -6523,7 +7066,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A12" s="5" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>182</v>
@@ -6631,7 +7174,7 @@
         <v>182</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>63</v>
@@ -6699,7 +7242,7 @@
         <v>182</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>67</v>
@@ -6716,7 +7259,7 @@
         <v>182</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>68</v>
@@ -6784,7 +7327,7 @@
         <v>181</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>72</v>
@@ -6869,7 +7412,7 @@
         <v>183</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>77</v>
@@ -7056,7 +7599,7 @@
         <v>181</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>88</v>
@@ -7114,6 +7657,469 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A1A692-D277-4E49-B99B-31BF1B967374}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="52.86328125" customWidth="1"/>
+    <col min="2" max="2" width="56.58984375" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.54296875" customWidth="1"/>
+    <col min="5" max="5" width="42.90625" customWidth="1"/>
+    <col min="6" max="6" width="15.58984375" customWidth="1"/>
+    <col min="7" max="7" width="11.1328125" customWidth="1"/>
+    <col min="8" max="8" width="64.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A2" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A2</f>
+        <v>Alerts.allergy</v>
+      </c>
+      <c r="D2" s="5" t="str">
+        <f>[1]AlertsEhn!D2</f>
+        <v>A.2.2.1 - Allergy and Intolerance</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>684</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A3" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A2</f>
+        <v>Alerts.allergy</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <f>[1]AlertsEhn!D2</f>
+        <v>A.2.2.1 - Allergy and Intolerance</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>686</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A4" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A3</f>
+        <v>Alerts.allergy.description</v>
+      </c>
+      <c r="D4" s="5" t="str">
+        <f>[1]AlertsEhn!D3</f>
+        <v>A.2.2.1.1 - Allergy description</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>688</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A5" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A4</f>
+        <v>Alerts.allergy.typeOfPropensity</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <f>[1]AlertsEhn!D4</f>
+        <v>A.2.2.1.2 - Type of propensity</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>689</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A6" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C6" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A5</f>
+        <v>Alerts.allergy.manifestation</v>
+      </c>
+      <c r="D6" s="5" t="str">
+        <f>[1]AlertsEhn!D5</f>
+        <v>A.2.2.1.3 - Allergy manifestation</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>690</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A7" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A5</f>
+        <v>Alerts.allergy.manifestation</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <f>[1]AlertsEhn!D5</f>
+        <v>A.2.2.1.3 - Allergy manifestation</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>691</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A8" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C8" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A6</f>
+        <v>Alerts.allergy.severity</v>
+      </c>
+      <c r="D8" s="5" t="str">
+        <f>[1]AlertsEhn!D6</f>
+        <v>A.2.2.1.4 - Severity</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A9" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A7</f>
+        <v>Alerts.allergy.criticality</v>
+      </c>
+      <c r="D9" s="5" t="str">
+        <f>[1]AlertsEhn!D7</f>
+        <v>A.2.2.1.5 - Criticality</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A10" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C10" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A8</f>
+        <v>Alerts.allergy.onsetDate</v>
+      </c>
+      <c r="D10" s="5" t="str">
+        <f>[1]AlertsEhn!D8</f>
+        <v>A.2.2.1.6 - Onset date</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A11" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A11</f>
+        <v>Alerts.allergy.endDate</v>
+      </c>
+      <c r="D11" s="5" t="str">
+        <f>[1]AlertsEhn!D11</f>
+        <v>A.2.2.1.7 - End date</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>695</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A12" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C12" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A14</f>
+        <v>Alerts.allergy.status</v>
+      </c>
+      <c r="D12" s="5" t="str">
+        <f>[1]AlertsEhn!D14</f>
+        <v>A.2.2.1.8 - Status</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A13" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A15</f>
+        <v>Alerts.allergy.certainty</v>
+      </c>
+      <c r="D13" s="5" t="str">
+        <f>[1]AlertsEhn!D15</f>
+        <v>A.2.2.1.9 - Certainty</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A14" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="C14" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A16</f>
+        <v>Alerts.allergy.agent</v>
+      </c>
+      <c r="D14" s="5" t="str">
+        <f>[1]AlertsEhn!D16</f>
+        <v>A.2.2.1.10 - Agent or Allergen</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>698</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A15" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>703</v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A17</f>
+        <v>Alerts.medicalAlerts</v>
+      </c>
+      <c r="D15" s="5" t="str">
+        <f>[1]AlertsEhn!D17</f>
+        <v>A.2.2.2 - Medical alerts (relevant for the respective hospital stay)</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>699</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A16" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>703</v>
+      </c>
+      <c r="C16" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A18</f>
+        <v>Alerts.medicalAlerts.description</v>
+      </c>
+      <c r="D16" s="5" t="str">
+        <f>[1]AlertsEhn!D18</f>
+        <v>A.2.2.2.1 - Healthcare alert description</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A17" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>706</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A18</f>
+        <v>Alerts.medicalAlerts.description</v>
+      </c>
+      <c r="D17" s="5" t="str">
+        <f>[1]AlertsEhn!D18</f>
+        <v>A.2.2.2.1 - Healthcare alert description</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>701</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A18" s="8" t="s">
+        <v>705</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>706</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f>"Alerts."&amp;[1]AlertsEhn!A18</f>
+        <v>Alerts.medicalAlerts.description</v>
+      </c>
+      <c r="D18" s="5" t="str">
+        <f>[1]AlertsEhn!D18</f>
+        <v>A.2.2.2.1 - Healthcare alert description</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>702</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="H18" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{BCEC97F6-9335-434E-99C2-DA2C9624174D}"/>
+    <hyperlink ref="A2" r:id="rId2" display="http://hl7.eu/fhir/eps/StructureDefinition/Alerts2FHIREuEps" xr:uid="{4950001C-E6D9-4E8F-ACEE-F8A8FA36F96E}"/>
+    <hyperlink ref="A4:A17" r:id="rId3" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{4847A3E0-CDC5-43BF-AFFD-11EDCA924FB2}"/>
+    <hyperlink ref="B3" r:id="rId4" display="http://hl7.eu/fhir/hdr/StructureDefinition/allergyIntolerance-eu-hdr" xr:uid="{8FA1E2F3-8B54-4819-8378-4D5A29863A0B}"/>
+    <hyperlink ref="A3" r:id="rId5" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{F4F2523C-3BC8-49E1-99E3-DFFC2E7596CB}"/>
+    <hyperlink ref="A6" r:id="rId6" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{6649B259-26A2-4108-B5AA-71477463F534}"/>
+    <hyperlink ref="B17" r:id="rId7" xr:uid="{012242A9-1402-4E3C-BC89-9DDAEAD17100}"/>
+    <hyperlink ref="B15" r:id="rId8" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{3C130F49-1368-40F8-919F-3DEDF3E91A6E}"/>
+    <hyperlink ref="A16" r:id="rId9" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{9F283B31-0F43-4146-A80A-E7064B87960C}"/>
+    <hyperlink ref="B16" r:id="rId10" display="http://hl7.eu/fhir/hdr/StructureDefinition/composition-eu-hdr" xr:uid="{46D4BACE-90A0-49D1-BCE1-CC158EEA1685}"/>
+    <hyperlink ref="A18" r:id="rId11" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{DD18BC4B-97C7-4AD8-818C-30415EE2C9E5}"/>
+    <hyperlink ref="B18" r:id="rId12" xr:uid="{043ABC1F-1A92-452B-ABD2-CD7D89F98B88}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
@@ -7316,7 +8322,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
@@ -7417,7 +8423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
@@ -7518,7 +8524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -7631,187 +8637,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D2" t="s">
-        <v>306</v>
-      </c>
-      <c r="E2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>292</v>
-      </c>
-      <c r="B3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D3" t="s">
-        <v>307</v>
-      </c>
-      <c r="E3" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>293</v>
-      </c>
-      <c r="B4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D4" t="s">
-        <v>308</v>
-      </c>
-      <c r="E4" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>294</v>
-      </c>
-      <c r="B5" t="s">
-        <v>299</v>
-      </c>
-      <c r="C5" t="s">
-        <v>184</v>
-      </c>
-      <c r="D5" t="s">
-        <v>309</v>
-      </c>
-      <c r="E5" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>295</v>
-      </c>
-      <c r="B6" t="s">
-        <v>300</v>
-      </c>
-      <c r="C6" t="s">
-        <v>305</v>
-      </c>
-      <c r="D6" t="s">
-        <v>310</v>
-      </c>
-      <c r="E6" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
-        <v>296</v>
-      </c>
-      <c r="B7" t="s">
-        <v>301</v>
-      </c>
-      <c r="C7" t="s">
-        <v>187</v>
-      </c>
-      <c r="D7" t="s">
-        <v>311</v>
-      </c>
-      <c r="E7" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>297</v>
-      </c>
-      <c r="B8" t="s">
-        <v>302</v>
-      </c>
-      <c r="C8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D8" t="s">
-        <v>312</v>
-      </c>
-      <c r="E8" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>298</v>
-      </c>
-      <c r="B9" t="s">
-        <v>303</v>
-      </c>
-      <c r="C9" t="s">
-        <v>187</v>
-      </c>
-      <c r="D9" t="s">
-        <v>313</v>
-      </c>
-      <c r="E9" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
-        <v>234</v>
-      </c>
-      <c r="B10" t="s">
-        <v>304</v>
-      </c>
-      <c r="C10" t="s">
-        <v>186</v>
-      </c>
-      <c r="D10" t="s">
-        <v>314</v>
-      </c>
-      <c r="E10" t="s">
-        <v>323</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
partial realignment with the new base ig
</commit_message>
<xml_diff>
--- a/models-src/hl7-eps-models-and-maps.xlsx
+++ b/models-src/hl7-eps-models-and-maps.xlsx
@@ -1,42 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\hl7eu-eps\models-src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC2F38C0-10F5-4A88-AF72-B2DC27F9481F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA085BBA-5132-42C5-9653-49DBA57F839F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-21710" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConceptMaps" sheetId="15" r:id="rId1"/>
-    <sheet name="PatientSummary2FHIR" sheetId="1" r:id="rId2"/>
-    <sheet name="PatientSummarySubject2Fhir" sheetId="14" r:id="rId3"/>
-    <sheet name="PatientSummaryEhn" sheetId="2" r:id="rId4"/>
-    <sheet name="Alerts2FHIREuHdr" sheetId="17" r:id="rId5"/>
-    <sheet name="AllergyPsEhn" sheetId="3" r:id="rId6"/>
-    <sheet name="ClosedProblemPsEhn" sheetId="4" r:id="rId7"/>
-    <sheet name="MedicalDevicePsEhn" sheetId="5" r:id="rId8"/>
-    <sheet name="FunctionalStatusPsEhn" sheetId="6" r:id="rId9"/>
-    <sheet name="MedicinePsEhn" sheetId="7" r:id="rId10"/>
-    <sheet name="PregnancyPsEhn" sheetId="8" r:id="rId11"/>
-    <sheet name="ProblemPsEhn" sheetId="9" r:id="rId12"/>
-    <sheet name="ProcedurePsEhn" sheetId="10" r:id="rId13"/>
-    <sheet name="ResultPsEhn" sheetId="11" r:id="rId14"/>
-    <sheet name="SubjectPsEhn" sheetId="12" r:id="rId15"/>
-    <sheet name="VaccinationPsEhn" sheetId="13" r:id="rId16"/>
-    <sheet name="LogicalModels" sheetId="16" r:id="rId17"/>
+    <sheet name="LogicalModels" sheetId="16" r:id="rId2"/>
+    <sheet name="Vaccination2FHIRPs" sheetId="18" r:id="rId3"/>
+    <sheet name="VaccinationPsEhn" sheetId="13" r:id="rId4"/>
+    <sheet name="PatientSummary2FHIR" sheetId="1" r:id="rId5"/>
+    <sheet name="PatientSummarySubject2Fhir" sheetId="14" r:id="rId6"/>
+    <sheet name="PatientSummaryEhn" sheetId="2" r:id="rId7"/>
+    <sheet name="Alerts2FHIREuHdr" sheetId="17" r:id="rId8"/>
+    <sheet name="AllergyPsEhn" sheetId="3" r:id="rId9"/>
+    <sheet name="ClosedProblemPsEhn" sheetId="4" r:id="rId10"/>
+    <sheet name="MedicalDevicePsEhn" sheetId="5" r:id="rId11"/>
+    <sheet name="FunctionalStatusPsEhn" sheetId="6" r:id="rId12"/>
+    <sheet name="MedicinePsEhn" sheetId="7" r:id="rId13"/>
+    <sheet name="PregnancyPsEhn" sheetId="8" r:id="rId14"/>
+    <sheet name="ProblemPsEhn" sheetId="9" r:id="rId15"/>
+    <sheet name="ProcedurePsEhn" sheetId="10" r:id="rId16"/>
+    <sheet name="ResultPsEhn" sheetId="11" r:id="rId17"/>
+    <sheet name="SubjectPsEhn" sheetId="12" r:id="rId18"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId18"/>
     <externalReference r:id="rId19"/>
+    <externalReference r:id="rId20"/>
   </externalReferences>
   <definedNames>
-    <definedName name="CENEN13606Lekarska_prepustacia_sprava">'[2]Hospital Discharge Report '!#REF!</definedName>
+    <definedName name="CENEN13606Lekarska_prepustacia_sprava">'[1]Hospital Discharge Report '!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1563" uniqueCount="723">
   <si>
     <t>Group Source</t>
   </si>
@@ -2192,6 +2193,54 @@
   </si>
   <si>
     <t>http://hl7.eu/fhir/hdr/StructureDefinition/flag-eu-eps</t>
+  </si>
+  <si>
+    <t>Immunization.protocolApplied.targetDisease</t>
+  </si>
+  <si>
+    <t>Immunization.vaccineCode</t>
+  </si>
+  <si>
+    <t>Immunization.extension:administeredProduct</t>
+  </si>
+  <si>
+    <t>Immunization.manufacturer</t>
+  </si>
+  <si>
+    <t>Immunization.protocolApplied.doseNumberPositiveInt</t>
+  </si>
+  <si>
+    <t>Immunization.occurenceDateTime</t>
+  </si>
+  <si>
+    <t>ImmunizationRecommendation.recommendation.dateCriterion[nextDose].value</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/eps/StructureDefinition/immunization-eu-eps</t>
+  </si>
+  <si>
+    <t>add more specific target</t>
+  </si>
+  <si>
+    <t>Immunization.lotNumber</t>
+  </si>
+  <si>
+    <t>Immunization.performer:administeringCentre</t>
+  </si>
+  <si>
+    <t>Immunization.performer:administeringHp.identifier</t>
+  </si>
+  <si>
+    <t>Immunization.location.address.country</t>
+  </si>
+  <si>
+    <t>http://hl7.eu/fhir/eps/StructureDefinition/ImmunizationRecommendation-eu-eps</t>
+  </si>
+  <si>
+    <t>Vaccination2FHIRPs</t>
+  </si>
+  <si>
+    <t>vaccination2FHIR-eu-eps</t>
   </si>
 </sst>
 </file>
@@ -2250,7 +2299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2286,6 +2335,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2294,7 +2367,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2325,6 +2398,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -2350,8 +2428,106 @@
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
+      <sheetName val="Hospital Discharge Report "/>
+      <sheetName val="HospitalDischargeReport"/>
+      <sheetName val="HospitalDischargeReport-Map-1"/>
+      <sheetName val="HospitalDischargeReport-fsh"/>
+      <sheetName val="HospitalDischargeRep-ConceptMap"/>
+      <sheetName val="HospitalDischargeReport-CM-fsh"/>
+      <sheetName val="HDR-SK"/>
+      <sheetName val="HospitalDischargeReportSK"/>
+      <sheetName val="HospitalDischargeReportSK-Map"/>
+      <sheetName val="HospitalDischargeReportSK-fsh"/>
+      <sheetName val="Subject"/>
+      <sheetName val="Subject-Map-1"/>
+      <sheetName val="Subject-fsh"/>
+      <sheetName val="Subject-ConceptMap"/>
+      <sheetName val="Subject-CM-fsh"/>
+      <sheetName val="Staging"/>
+      <sheetName val="Staging-Map-1"/>
+      <sheetName val="Staging-fsh"/>
+      <sheetName val="Staging-ConceptMap"/>
+      <sheetName val="Staging-CM-fsh"/>
+      <sheetName val="Treatment"/>
+      <sheetName val="Treatment-Map-1"/>
+      <sheetName val="Treatment-fsh"/>
+      <sheetName val="Treatment-ConceptMap"/>
+      <sheetName val="Treatment-CM-fsh"/>
+      <sheetName val="ConvertOsiris"/>
+      <sheetName val="Osiris"/>
+      <sheetName val="Osiris-Map"/>
+      <sheetName val="Osiris-fsh-noMap"/>
+      <sheetName val="Osiris-fsh"/>
+      <sheetName val="Osiris-ConceptMap"/>
+      <sheetName val="Osiris-CM-fsh"/>
+      <sheetName val="Foglio2"/>
+      <sheetName val="xpandh-hdr-model-maps"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="IG-groups"/>
       <sheetName val="ConceptMaps"/>
       <sheetName val="LogicalModels"/>
+      <sheetName val="PatientHistory2FHIREuHdr"/>
+      <sheetName val="PatientHistoryEhn"/>
+      <sheetName val="HospitalStay2FHIREuHdr"/>
+      <sheetName val="HospitalStayEhn"/>
+      <sheetName val="Hdr2FHIREuHdr"/>
+      <sheetName val="HospitalDischargeReportEhn"/>
+      <sheetName val="ObjectiveFindingsHdrEhn"/>
+      <sheetName val="FunctionalStatus2FHIREuHdr"/>
+      <sheetName val="FunctionalStatusHdrEhn"/>
+      <sheetName val="MedicationSummary2FHIREuHdr"/>
+      <sheetName val="MedicationSummaryHdrEhn"/>
+      <sheetName val="PlanOfCare2FHIREuHdr"/>
+      <sheetName val="PlanOfCareHdrEhn"/>
+      <sheetName val="AdvanceDirectives2FHIREuHdr"/>
+      <sheetName val="AdvanceDirectivesEhn"/>
       <sheetName val="Alerts2FHIREuHdr"/>
       <sheetName val="AlertsEhn"/>
       <sheetName val="Encounter2FHIREuHdr"/>
@@ -2360,19 +2536,29 @@
       <sheetName val="Subject2FHIREuHdr"/>
       <sheetName val="SubjectHdrEhn"/>
       <sheetName val="AdmissionEvaluationEhn"/>
-      <sheetName val="AdvanceDirectivesEhn"/>
-      <sheetName val="DischargeDetailsEhn"/>
       <sheetName val="EncounterEhn"/>
-      <sheetName val="HospitalStayEhn"/>
-      <sheetName val="PatientHistoryEhn"/>
-      <sheetName val="RecommendationsEhn"/>
-      <sheetName val="HospitalDischargeReportEhn"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19">
         <row r="2">
           <cell r="A2" t="str">
             <v>allergy</v>
@@ -2478,101 +2664,13 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Hospital Discharge Report "/>
-      <sheetName val="HospitalDischargeReport"/>
-      <sheetName val="HospitalDischargeReport-Map-1"/>
-      <sheetName val="HospitalDischargeReport-fsh"/>
-      <sheetName val="HospitalDischargeRep-ConceptMap"/>
-      <sheetName val="HospitalDischargeReport-CM-fsh"/>
-      <sheetName val="HDR-SK"/>
-      <sheetName val="HospitalDischargeReportSK"/>
-      <sheetName val="HospitalDischargeReportSK-Map"/>
-      <sheetName val="HospitalDischargeReportSK-fsh"/>
-      <sheetName val="Subject"/>
-      <sheetName val="Subject-Map-1"/>
-      <sheetName val="Subject-fsh"/>
-      <sheetName val="Subject-ConceptMap"/>
-      <sheetName val="Subject-CM-fsh"/>
-      <sheetName val="Staging"/>
-      <sheetName val="Staging-Map-1"/>
-      <sheetName val="Staging-fsh"/>
-      <sheetName val="Staging-ConceptMap"/>
-      <sheetName val="Staging-CM-fsh"/>
-      <sheetName val="Treatment"/>
-      <sheetName val="Treatment-Map-1"/>
-      <sheetName val="Treatment-fsh"/>
-      <sheetName val="Treatment-ConceptMap"/>
-      <sheetName val="Treatment-CM-fsh"/>
-      <sheetName val="ConvertOsiris"/>
-      <sheetName val="Osiris"/>
-      <sheetName val="Osiris-Map"/>
-      <sheetName val="Osiris-fsh-noMap"/>
-      <sheetName val="Osiris-fsh"/>
-      <sheetName val="Osiris-ConceptMap"/>
-      <sheetName val="Osiris-CM-fsh"/>
-      <sheetName val="Foglio2"/>
-      <sheetName val="xpandh-hdr-model-maps"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2871,7 +2969,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2981,7 +3079,7 @@
         <v>681</v>
       </c>
       <c r="C4" s="8" t="str">
-        <f t="shared" ref="C4" si="0">"http://hl7.eu/fhir/hdr/ConceptMap/"&amp;A4</f>
+        <f t="shared" ref="C4:C5" si="0">"http://hl7.eu/fhir/hdr/ConceptMap/"&amp;A4</f>
         <v>http://hl7.eu/fhir/hdr/ConceptMap/alerts2FHIR-eu-eps</v>
       </c>
       <c r="D4" s="5" t="s">
@@ -3002,6 +3100,40 @@
       <c r="I4" s="13" t="s">
         <v>676</v>
       </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A5" s="13" t="s">
+        <v>722</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="C5" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.eu/fhir/hdr/ConceptMap/vaccination2FHIR-eu-eps</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>674</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="G5" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!A13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="A8" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.75">
       <c r="C12" s="1"/>
@@ -3009,18 +3141,339 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="http://hl7.eu/fhir/ig/xpandh/ps/StructureDefinition/PatientSummary" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
-    <hyperlink ref="G3" r:id="rId2" display="http://hl7.eu/fhir/ig/xpandh/ps/StructureDefinition/Subject" xr:uid="{00000000-0004-0000-0E00-000004000000}"/>
-    <hyperlink ref="C2" r:id="rId3" display="http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId4" display="http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR" xr:uid="{0041CA32-1BC1-4938-801E-686765723E3F}"/>
-    <hyperlink ref="C4" r:id="rId5" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{42BB9F16-F29B-4D9B-A55C-529961F089C2}"/>
-    <hyperlink ref="H4" r:id="rId6" xr:uid="{D0CFA2F1-ED0F-4899-907A-300DECE34DC2}"/>
-    <hyperlink ref="G4" r:id="rId7" xr:uid="{D6CB4B67-C29F-4503-B9BB-BD22D2DA2E6F}"/>
+    <hyperlink ref="C2" r:id="rId2" display="http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId3" display="http://hl7.eu/fhir/eps/ConceptMap/patientSummary2FHIR" xr:uid="{0041CA32-1BC1-4938-801E-686765723E3F}"/>
+    <hyperlink ref="C4" r:id="rId4" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{42BB9F16-F29B-4D9B-A55C-529961F089C2}"/>
+    <hyperlink ref="H4" r:id="rId5" xr:uid="{D0CFA2F1-ED0F-4899-907A-300DECE34DC2}"/>
+    <hyperlink ref="B5" location="Vaccination2FHIRPs!A1" display="Vaccination2FHIRPs" xr:uid="{84D17118-9CF9-4786-8EC5-09FA66190CFC}"/>
+    <hyperlink ref="C5" r:id="rId6" display="http://terminology.hl7.it/ConceptMap/ConceptMap-subject2osiris" xr:uid="{5451B0A8-737F-4B98-8412-27A43B025DED}"/>
+    <hyperlink ref="H5" r:id="rId7" xr:uid="{A61A4DA4-0D65-4BBE-9B9F-0A5EA9C207B8}"/>
+    <hyperlink ref="G5" r:id="rId8" display="http://hl7.eu/fhir/eps/StructureDefinition/Alert" xr:uid="{9F946528-2C63-4603-ABCD-0A537B3D6067}"/>
+    <hyperlink ref="G3" r:id="rId9" display="http://hl7.eu/fhir/ig/xpandh/ps/StructureDefinition/Subject" xr:uid="{00000000-0004-0000-0E00-000004000000}"/>
+    <hyperlink ref="G4" r:id="rId10" xr:uid="{D6CB4B67-C29F-4503-B9BB-BD22D2DA2E6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>259</v>
+      </c>
+      <c r="B5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" t="s">
+        <v>263</v>
+      </c>
+      <c r="E5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E5" t="s">
+        <v>277</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" t="s">
+        <v>283</v>
+      </c>
+      <c r="E4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" t="s">
+        <v>284</v>
+      </c>
+      <c r="E5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" t="s">
+        <v>285</v>
+      </c>
+      <c r="E6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -3203,7 +3656,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -3403,7 +3856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3484,7 +3937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -3565,7 +4018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -3731,7 +4184,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
@@ -4288,246 +4741,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:E13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>477</v>
-      </c>
-      <c r="B2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D2" t="s">
-        <v>489</v>
-      </c>
-      <c r="E2" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>478</v>
-      </c>
-      <c r="B3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D3" t="s">
-        <v>490</v>
-      </c>
-      <c r="E3" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>293</v>
-      </c>
-      <c r="B4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D4" t="s">
-        <v>491</v>
-      </c>
-      <c r="E4" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>479</v>
-      </c>
-      <c r="B5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D5" t="s">
-        <v>492</v>
-      </c>
-      <c r="E5" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>480</v>
-      </c>
-      <c r="B6" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" t="s">
-        <v>493</v>
-      </c>
-      <c r="E6" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
-        <v>481</v>
-      </c>
-      <c r="B7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C7" t="s">
-        <v>184</v>
-      </c>
-      <c r="D7" t="s">
-        <v>494</v>
-      </c>
-      <c r="E7" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>482</v>
-      </c>
-      <c r="B8" t="s">
-        <v>182</v>
-      </c>
-      <c r="C8" t="s">
-        <v>189</v>
-      </c>
-      <c r="D8" t="s">
-        <v>495</v>
-      </c>
-      <c r="E8" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>483</v>
-      </c>
-      <c r="B9" t="s">
-        <v>182</v>
-      </c>
-      <c r="C9" t="s">
-        <v>186</v>
-      </c>
-      <c r="D9" t="s">
-        <v>496</v>
-      </c>
-      <c r="E9" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
-        <v>484</v>
-      </c>
-      <c r="B10" t="s">
-        <v>182</v>
-      </c>
-      <c r="C10" t="s">
-        <v>488</v>
-      </c>
-      <c r="D10" t="s">
-        <v>497</v>
-      </c>
-      <c r="E10" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
-        <v>485</v>
-      </c>
-      <c r="B11" t="s">
-        <v>182</v>
-      </c>
-      <c r="C11" t="s">
-        <v>268</v>
-      </c>
-      <c r="D11" t="s">
-        <v>498</v>
-      </c>
-      <c r="E11" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
-        <v>486</v>
-      </c>
-      <c r="B12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C12" t="s">
-        <v>187</v>
-      </c>
-      <c r="D12" t="s">
-        <v>499</v>
-      </c>
-      <c r="E12" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A13" t="s">
-        <v>487</v>
-      </c>
-      <c r="B13" t="s">
-        <v>182</v>
-      </c>
-      <c r="C13" t="s">
-        <v>186</v>
-      </c>
-      <c r="D13" t="s">
-        <v>500</v>
-      </c>
-      <c r="E13" t="s">
-        <v>512</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4710,7 +4929,7 @@
       <c r="A13" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="8" t="s">
         <v>620</v>
       </c>
       <c r="C13" s="5" t="s">
@@ -4723,19 +4942,623 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" location="PatientSummaryEhn!A1" display="PatientSummaryEhn" xr:uid="{5021AE86-C78E-4794-8FB8-7E3E7942E3EA}"/>
+    <hyperlink ref="B13" location="VaccinationPsEhn!A1" display="VaccinationPsEhn" xr:uid="{FC860359-0D35-409E-854F-C1BE7C75509B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE95AB6E-9619-4905-B2ED-C9E2B9BD8545}">
+  <sheetPr>
+    <tabColor theme="3" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="1" max="1" width="52.86328125" customWidth="1"/>
+    <col min="2" max="2" width="56.58984375" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.54296875" customWidth="1"/>
+    <col min="5" max="5" width="42.90625" customWidth="1"/>
+    <col min="6" max="6" width="15.58984375" customWidth="1"/>
+    <col min="7" max="7" width="11.1328125" customWidth="1"/>
+    <col min="8" max="8" width="64.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A2" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A2</f>
+        <v>Vaccination.targetDisease</v>
+      </c>
+      <c r="D2" s="5" t="str">
+        <f>VaccinationPsEhn!D2</f>
+        <v>A.2.2.1.1 Disease or agent targeted</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A3" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A3</f>
+        <v>Vaccination.vaccine</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <f>VaccinationPsEhn!D3</f>
+        <v>A.2.2.1.2 Vaccine/prophylaxis</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A4" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A4</f>
+        <v>Vaccination.productName</v>
+      </c>
+      <c r="D4" s="5" t="str">
+        <f>VaccinationPsEhn!D4</f>
+        <v>A.2.2.1.3 Vaccine medicinal product name</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A5" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A5</f>
+        <v>Vaccination.productId</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <f>VaccinationPsEhn!D5</f>
+        <v>A.2.2.1.3.1 Identifier of the vaccine medicinal product</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>709</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="12" t="s">
+        <v>685</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A6" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="C6" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A6</f>
+        <v>Vaccination.marketingAuthorisationHolder</v>
+      </c>
+      <c r="D6" s="5" t="str">
+        <f>VaccinationPsEhn!D6</f>
+        <v>A.2.2.1.4 Marketing Autorisation Holder</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>710</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A7" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A7</f>
+        <v>Vaccination.numberInSeries</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <f>VaccinationPsEhn!D7</f>
+        <v>A.2.2.1.5 Number in a series of vaccinations/doses</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>711</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>685</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A8" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="C8" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A8</f>
+        <v>Vaccination.batchNumber</v>
+      </c>
+      <c r="D8" s="5" t="str">
+        <f>VaccinationPsEhn!D8</f>
+        <v>A.2.2.1.6 Batch/lot number</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>716</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="18" t="s">
+        <v>685</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A9" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A9</f>
+        <v>Vaccination.dateOfVaccination</v>
+      </c>
+      <c r="D9" s="5" t="str">
+        <f>VaccinationPsEhn!D9</f>
+        <v>A.2.2.1.7 Date of vaccination</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>712</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="18" t="s">
+        <v>685</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A10" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="C10" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A10</f>
+        <v>Vaccination.administeringCentre</v>
+      </c>
+      <c r="D10" s="5" t="str">
+        <f>VaccinationPsEhn!D10</f>
+        <v>A.2.2.1.8 Administering centre</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>717</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="18" t="s">
+        <v>685</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A11" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A11</f>
+        <v>Vaccination.healthProfessionalId</v>
+      </c>
+      <c r="D11" s="5" t="str">
+        <f>VaccinationPsEhn!D11</f>
+        <v>A.2.2.1.9 Health Professional identification</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>718</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="18" t="s">
+        <v>685</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.75">
+      <c r="A12" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="C12" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A12</f>
+        <v>Vaccination.countryOfVaccination</v>
+      </c>
+      <c r="D12" s="5" t="str">
+        <f>VaccinationPsEhn!D12</f>
+        <v>A.2.2.1.10 Country of vaccination</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="18" t="s">
+        <v>685</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="29.5" x14ac:dyDescent="0.75">
+      <c r="A13" s="8" t="str">
+        <f>"http://hl7.eu/fhir/eps/StructureDefinition/"&amp;LogicalModels!$A$13</f>
+        <v>http://hl7.eu/fhir/eps/StructureDefinition/Vaccination</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>720</v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <f>LogicalModels!$A$13&amp;"."&amp;VaccinationPsEhn!A13</f>
+        <v>Vaccination.dateOfNextVaccination</v>
+      </c>
+      <c r="D13" s="5" t="str">
+        <f>VaccinationPsEhn!D13</f>
+        <v>A.2.2.1.11 Next vaccination date</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>713</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="18" t="s">
+        <v>685</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{0FF3177F-82D6-4AAD-91D7-ED272A5FE9A2}"/>
+    <hyperlink ref="A2" r:id="rId2" display="http://hl7.eu/fhir/eps/StructureDefinition/Alerts" xr:uid="{F301213C-EC18-48A0-9B04-2DA772B0E5DD}"/>
+    <hyperlink ref="A4:A13" r:id="rId3" display="http://hl7.eu/fhir/hdr/StructureDefinition/Alerts2FHIREuHdr" xr:uid="{CE6196DC-ED70-4AEE-8BD1-A566EDDEB831}"/>
+    <hyperlink ref="A3:A13" r:id="rId4" display="http://hl7.eu/fhir/eps/StructureDefinition/Alerts" xr:uid="{1C4EC159-5F45-4441-976E-61286ADD71E0}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{CE04BD9A-6452-48CA-90D7-1B31A755BAB4}"/>
+    <hyperlink ref="B13" r:id="rId6" xr:uid="{1A291BEB-19D8-4DAC-8504-AB5B20AC1EFA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>477</v>
+      </c>
+      <c r="B2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" t="s">
+        <v>489</v>
+      </c>
+      <c r="E2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>478</v>
+      </c>
+      <c r="B3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" t="s">
+        <v>490</v>
+      </c>
+      <c r="E3" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" t="s">
+        <v>491</v>
+      </c>
+      <c r="E4" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>479</v>
+      </c>
+      <c r="B5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" t="s">
+        <v>492</v>
+      </c>
+      <c r="E5" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>480</v>
+      </c>
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" t="s">
+        <v>493</v>
+      </c>
+      <c r="E6" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>481</v>
+      </c>
+      <c r="B7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" t="s">
+        <v>494</v>
+      </c>
+      <c r="E7" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>482</v>
+      </c>
+      <c r="B8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" t="s">
+        <v>495</v>
+      </c>
+      <c r="E8" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>483</v>
+      </c>
+      <c r="B9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" t="s">
+        <v>496</v>
+      </c>
+      <c r="E9" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>484</v>
+      </c>
+      <c r="B10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" t="s">
+        <v>488</v>
+      </c>
+      <c r="D10" t="s">
+        <v>497</v>
+      </c>
+      <c r="E10" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>485</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" t="s">
+        <v>268</v>
+      </c>
+      <c r="D11" t="s">
+        <v>498</v>
+      </c>
+      <c r="E11" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>486</v>
+      </c>
+      <c r="B12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" t="s">
+        <v>499</v>
+      </c>
+      <c r="E12" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>487</v>
+      </c>
+      <c r="B13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" t="s">
+        <v>500</v>
+      </c>
+      <c r="E13" t="s">
+        <v>512</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView topLeftCell="C18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -5995,7 +6818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
@@ -6857,7 +7680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
@@ -7656,14 +8479,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A1A692-D277-4E49-B99B-31BF1B967374}">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -7713,11 +8536,11 @@
         <v>703</v>
       </c>
       <c r="C2" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A2</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A2</f>
         <v>Alerts.allergy</v>
       </c>
       <c r="D2" s="5" t="str">
-        <f>[1]AlertsEhn!D2</f>
+        <f>[2]AlertsEhn!D2</f>
         <v>A.2.2.1 - Allergy and Intolerance</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -7736,11 +8559,11 @@
         <v>704</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A2</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A2</f>
         <v>Alerts.allergy</v>
       </c>
       <c r="D3" s="5" t="str">
-        <f>[1]AlertsEhn!D2</f>
+        <f>[2]AlertsEhn!D2</f>
         <v>A.2.2.1 - Allergy and Intolerance</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -7759,11 +8582,11 @@
         <v>704</v>
       </c>
       <c r="C4" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A3</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A3</f>
         <v>Alerts.allergy.description</v>
       </c>
       <c r="D4" s="5" t="str">
-        <f>[1]AlertsEhn!D3</f>
+        <f>[2]AlertsEhn!D3</f>
         <v>A.2.2.1.1 - Allergy description</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -7782,11 +8605,11 @@
         <v>704</v>
       </c>
       <c r="C5" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A4</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A4</f>
         <v>Alerts.allergy.typeOfPropensity</v>
       </c>
       <c r="D5" s="5" t="str">
-        <f>[1]AlertsEhn!D4</f>
+        <f>[2]AlertsEhn!D4</f>
         <v>A.2.2.1.2 - Type of propensity</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -7805,11 +8628,11 @@
         <v>704</v>
       </c>
       <c r="C6" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A5</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A5</f>
         <v>Alerts.allergy.manifestation</v>
       </c>
       <c r="D6" s="5" t="str">
-        <f>[1]AlertsEhn!D5</f>
+        <f>[2]AlertsEhn!D5</f>
         <v>A.2.2.1.3 - Allergy manifestation</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -7828,11 +8651,11 @@
         <v>704</v>
       </c>
       <c r="C7" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A5</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A5</f>
         <v>Alerts.allergy.manifestation</v>
       </c>
       <c r="D7" s="5" t="str">
-        <f>[1]AlertsEhn!D5</f>
+        <f>[2]AlertsEhn!D5</f>
         <v>A.2.2.1.3 - Allergy manifestation</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -7851,11 +8674,11 @@
         <v>704</v>
       </c>
       <c r="C8" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A6</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A6</f>
         <v>Alerts.allergy.severity</v>
       </c>
       <c r="D8" s="5" t="str">
-        <f>[1]AlertsEhn!D6</f>
+        <f>[2]AlertsEhn!D6</f>
         <v>A.2.2.1.4 - Severity</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -7874,11 +8697,11 @@
         <v>704</v>
       </c>
       <c r="C9" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A7</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A7</f>
         <v>Alerts.allergy.criticality</v>
       </c>
       <c r="D9" s="5" t="str">
-        <f>[1]AlertsEhn!D7</f>
+        <f>[2]AlertsEhn!D7</f>
         <v>A.2.2.1.5 - Criticality</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -7897,11 +8720,11 @@
         <v>704</v>
       </c>
       <c r="C10" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A8</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A8</f>
         <v>Alerts.allergy.onsetDate</v>
       </c>
       <c r="D10" s="5" t="str">
-        <f>[1]AlertsEhn!D8</f>
+        <f>[2]AlertsEhn!D8</f>
         <v>A.2.2.1.6 - Onset date</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -7920,11 +8743,11 @@
         <v>704</v>
       </c>
       <c r="C11" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A11</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A11</f>
         <v>Alerts.allergy.endDate</v>
       </c>
       <c r="D11" s="5" t="str">
-        <f>[1]AlertsEhn!D11</f>
+        <f>[2]AlertsEhn!D11</f>
         <v>A.2.2.1.7 - End date</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -7943,11 +8766,11 @@
         <v>704</v>
       </c>
       <c r="C12" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A14</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A14</f>
         <v>Alerts.allergy.status</v>
       </c>
       <c r="D12" s="5" t="str">
-        <f>[1]AlertsEhn!D14</f>
+        <f>[2]AlertsEhn!D14</f>
         <v>A.2.2.1.8 - Status</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -7966,11 +8789,11 @@
         <v>704</v>
       </c>
       <c r="C13" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A15</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A15</f>
         <v>Alerts.allergy.certainty</v>
       </c>
       <c r="D13" s="5" t="str">
-        <f>[1]AlertsEhn!D15</f>
+        <f>[2]AlertsEhn!D15</f>
         <v>A.2.2.1.9 - Certainty</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -7989,11 +8812,11 @@
         <v>704</v>
       </c>
       <c r="C14" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A16</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A16</f>
         <v>Alerts.allergy.agent</v>
       </c>
       <c r="D14" s="5" t="str">
-        <f>[1]AlertsEhn!D16</f>
+        <f>[2]AlertsEhn!D16</f>
         <v>A.2.2.1.10 - Agent or Allergen</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -8012,11 +8835,11 @@
         <v>703</v>
       </c>
       <c r="C15" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A17</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A17</f>
         <v>Alerts.medicalAlerts</v>
       </c>
       <c r="D15" s="5" t="str">
-        <f>[1]AlertsEhn!D17</f>
+        <f>[2]AlertsEhn!D17</f>
         <v>A.2.2.2 - Medical alerts (relevant for the respective hospital stay)</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -8035,11 +8858,11 @@
         <v>703</v>
       </c>
       <c r="C16" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A18</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A18</f>
         <v>Alerts.medicalAlerts.description</v>
       </c>
       <c r="D16" s="5" t="str">
-        <f>[1]AlertsEhn!D18</f>
+        <f>[2]AlertsEhn!D18</f>
         <v>A.2.2.2.1 - Healthcare alert description</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -8059,11 +8882,11 @@
         <v>706</v>
       </c>
       <c r="C17" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A18</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A18</f>
         <v>Alerts.medicalAlerts.description</v>
       </c>
       <c r="D17" s="5" t="str">
-        <f>[1]AlertsEhn!D18</f>
+        <f>[2]AlertsEhn!D18</f>
         <v>A.2.2.2.1 - Healthcare alert description</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -8083,11 +8906,11 @@
         <v>706</v>
       </c>
       <c r="C18" s="5" t="str">
-        <f>"Alerts."&amp;[1]AlertsEhn!A18</f>
+        <f>"Alerts."&amp;[2]AlertsEhn!A18</f>
         <v>Alerts.medicalAlerts.description</v>
       </c>
       <c r="D18" s="5" t="str">
-        <f>[1]AlertsEhn!D18</f>
+        <f>[2]AlertsEhn!D18</f>
         <v>A.2.2.2.1 - Healthcare alert description</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -8119,7 +8942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
@@ -8320,321 +9143,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr>
-    <tabColor theme="6" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" t="s">
-        <v>261</v>
-      </c>
-      <c r="E3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>235</v>
-      </c>
-      <c r="B4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D4" t="s">
-        <v>262</v>
-      </c>
-      <c r="E4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" t="s">
-        <v>187</v>
-      </c>
-      <c r="D5" t="s">
-        <v>263</v>
-      </c>
-      <c r="E5" t="s">
-        <v>267</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr>
-    <tabColor theme="6" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C2" t="s">
-        <v>187</v>
-      </c>
-      <c r="D2" t="s">
-        <v>270</v>
-      </c>
-      <c r="E2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>268</v>
-      </c>
-      <c r="B3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D3" t="s">
-        <v>271</v>
-      </c>
-      <c r="E3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>269</v>
-      </c>
-      <c r="B4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D5" t="s">
-        <v>273</v>
-      </c>
-      <c r="E5" t="s">
-        <v>277</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D3" t="s">
-        <v>282</v>
-      </c>
-      <c r="E3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>278</v>
-      </c>
-      <c r="B4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C4" t="s">
-        <v>187</v>
-      </c>
-      <c r="D4" t="s">
-        <v>283</v>
-      </c>
-      <c r="E4" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>279</v>
-      </c>
-      <c r="B5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C5" t="s">
-        <v>186</v>
-      </c>
-      <c r="D5" t="s">
-        <v>284</v>
-      </c>
-      <c r="E5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>280</v>
-      </c>
-      <c r="B6" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D6" t="s">
-        <v>285</v>
-      </c>
-      <c r="E6" t="s">
-        <v>290</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>